<commit_message>
Updated version of list
</commit_message>
<xml_diff>
--- a/stm/documents/algorithm_and_tests/Short_Variable_List_Sediment_Version_02_10_11_version_2.xlsx
+++ b/stm/documents/algorithm_and_tests/Short_Variable_List_Sediment_Version_02_10_11_version_2.xlsx
@@ -1559,7 +1559,7 @@
       <family val="1"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1569,6 +1569,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1720,7 +1726,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="34">
+  <cellXfs count="36">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1772,15 +1778,6 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1795,9 +1792,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1807,6 +1801,24 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2103,8 +2115,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:O56"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="F56" sqref="F56"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2140,45 +2152,45 @@
       <c r="O1" s="6"/>
     </row>
     <row r="2" spans="1:15" ht="132.75" customHeight="1">
-      <c r="B2" s="21" t="s">
+      <c r="B2" s="32" t="s">
         <v>133</v>
       </c>
-      <c r="C2" s="21"/>
-      <c r="D2" s="21"/>
-      <c r="E2" s="21"/>
-      <c r="F2" s="21"/>
-      <c r="G2" s="21"/>
-      <c r="H2" s="21"/>
-      <c r="I2" s="21"/>
-      <c r="J2" s="21"/>
-      <c r="K2" s="21"/>
-      <c r="L2" s="21"/>
-      <c r="M2" s="21"/>
-      <c r="N2" s="21"/>
-      <c r="O2" s="21"/>
+      <c r="C2" s="32"/>
+      <c r="D2" s="32"/>
+      <c r="E2" s="32"/>
+      <c r="F2" s="32"/>
+      <c r="G2" s="32"/>
+      <c r="H2" s="32"/>
+      <c r="I2" s="32"/>
+      <c r="J2" s="32"/>
+      <c r="K2" s="32"/>
+      <c r="L2" s="32"/>
+      <c r="M2" s="32"/>
+      <c r="N2" s="32"/>
+      <c r="O2" s="32"/>
     </row>
     <row r="3" spans="1:15" ht="19.5" thickBot="1">
-      <c r="A3" s="22" t="s">
+      <c r="A3" s="19" t="s">
         <v>93</v>
       </c>
-      <c r="B3" s="23"/>
-      <c r="C3" s="23"/>
-      <c r="D3" s="23"/>
+      <c r="B3" s="20"/>
+      <c r="C3" s="20"/>
+      <c r="D3" s="20"/>
     </row>
     <row r="4" spans="1:15" ht="25.5">
-      <c r="A4" s="24" t="s">
+      <c r="A4" s="21" t="s">
         <v>38</v>
       </c>
-      <c r="B4" s="25" t="s">
+      <c r="B4" s="22" t="s">
         <v>11</v>
       </c>
-      <c r="C4" s="25" t="s">
+      <c r="C4" s="22" t="s">
         <v>14</v>
       </c>
-      <c r="D4" s="25" t="s">
+      <c r="D4" s="22" t="s">
         <v>15</v>
       </c>
-      <c r="E4" s="26" t="s">
+      <c r="E4" s="23" t="s">
         <v>92</v>
       </c>
       <c r="F4" s="15"/>
@@ -2201,7 +2213,7 @@
       <c r="E5" s="10" t="s">
         <v>91</v>
       </c>
-      <c r="F5" s="4"/>
+      <c r="F5" s="33"/>
       <c r="G5" s="4"/>
       <c r="H5" s="4"/>
     </row>
@@ -2221,7 +2233,7 @@
       <c r="E6" s="10" t="s">
         <v>91</v>
       </c>
-      <c r="F6" s="19"/>
+      <c r="F6" s="34"/>
       <c r="G6" s="4"/>
       <c r="H6" s="4"/>
     </row>
@@ -2241,7 +2253,7 @@
       <c r="E7" s="10" t="s">
         <v>105</v>
       </c>
-      <c r="F7" s="4"/>
+      <c r="F7" s="33"/>
       <c r="G7" s="4"/>
       <c r="H7" s="4"/>
     </row>
@@ -2261,7 +2273,7 @@
       <c r="E8" s="10" t="s">
         <v>106</v>
       </c>
-      <c r="F8" s="4"/>
+      <c r="F8" s="33"/>
       <c r="G8" s="4"/>
       <c r="H8" s="4"/>
     </row>
@@ -2281,7 +2293,7 @@
       <c r="E9" s="10" t="s">
         <v>91</v>
       </c>
-      <c r="F9" s="4"/>
+      <c r="F9" s="33"/>
       <c r="G9" s="4"/>
       <c r="H9" s="4"/>
     </row>
@@ -2301,7 +2313,7 @@
       <c r="E10" s="10" t="s">
         <v>91</v>
       </c>
-      <c r="F10" s="4"/>
+      <c r="F10" s="33"/>
       <c r="G10" s="4"/>
       <c r="H10" s="4"/>
     </row>
@@ -2321,7 +2333,7 @@
       <c r="E11" s="10" t="s">
         <v>91</v>
       </c>
-      <c r="F11" s="4"/>
+      <c r="F11" s="33"/>
       <c r="G11" s="4"/>
       <c r="H11" s="4"/>
     </row>
@@ -2341,7 +2353,7 @@
       <c r="E12" s="10" t="s">
         <v>91</v>
       </c>
-      <c r="F12" s="4"/>
+      <c r="F12" s="33"/>
       <c r="G12" s="4"/>
       <c r="H12" s="4"/>
     </row>
@@ -2361,7 +2373,7 @@
       <c r="E13" s="8" t="s">
         <v>91</v>
       </c>
-      <c r="F13" s="9"/>
+      <c r="F13" s="33"/>
       <c r="G13" s="9"/>
       <c r="H13" s="9"/>
     </row>
@@ -2381,7 +2393,7 @@
       <c r="E14" s="8" t="s">
         <v>111</v>
       </c>
-      <c r="F14" s="9"/>
+      <c r="F14" s="33"/>
       <c r="G14" s="9"/>
       <c r="H14" s="9"/>
     </row>
@@ -2401,7 +2413,7 @@
       <c r="E15" s="8" t="s">
         <v>111</v>
       </c>
-      <c r="F15" s="9"/>
+      <c r="F15" s="33"/>
       <c r="G15" s="9"/>
       <c r="H15" s="9"/>
     </row>
@@ -2421,7 +2433,7 @@
       <c r="E16" s="8" t="s">
         <v>91</v>
       </c>
-      <c r="F16" s="9"/>
+      <c r="F16" s="33"/>
       <c r="G16" s="9"/>
       <c r="H16" s="9"/>
     </row>
@@ -2441,7 +2453,7 @@
       <c r="E17" s="8" t="s">
         <v>91</v>
       </c>
-      <c r="F17" s="9"/>
+      <c r="F17" s="33"/>
       <c r="G17" s="9"/>
       <c r="H17" s="9"/>
     </row>
@@ -2461,7 +2473,7 @@
       <c r="E18" s="10" t="s">
         <v>91</v>
       </c>
-      <c r="F18" s="4"/>
+      <c r="F18" s="33"/>
       <c r="G18" s="4"/>
       <c r="H18" s="4"/>
     </row>
@@ -2481,7 +2493,7 @@
       <c r="E19" s="10" t="s">
         <v>94</v>
       </c>
-      <c r="F19" s="4"/>
+      <c r="F19" s="35"/>
       <c r="G19" s="4"/>
       <c r="H19" s="4"/>
     </row>
@@ -2501,7 +2513,7 @@
       <c r="E20" s="10" t="s">
         <v>94</v>
       </c>
-      <c r="F20" s="4"/>
+      <c r="F20" s="35"/>
       <c r="G20" s="4"/>
       <c r="H20" s="4"/>
     </row>
@@ -2521,12 +2533,12 @@
       <c r="E21" s="10" t="s">
         <v>134</v>
       </c>
-      <c r="F21" s="4"/>
+      <c r="F21" s="35"/>
       <c r="G21" s="4"/>
       <c r="H21" s="4"/>
     </row>
     <row r="22" spans="1:8" ht="15.75" thickBot="1">
-      <c r="A22" s="27">
+      <c r="A22" s="24">
         <v>18</v>
       </c>
       <c r="B22" s="2" t="s">
@@ -2541,7 +2553,7 @@
       <c r="E22" s="14" t="s">
         <v>135</v>
       </c>
-      <c r="F22" s="4"/>
+      <c r="F22" s="35"/>
       <c r="G22" s="4"/>
       <c r="H22" s="4"/>
     </row>
@@ -2556,26 +2568,26 @@
       <c r="H23" s="4"/>
     </row>
     <row r="24" spans="1:8">
-      <c r="A24" s="20" t="s">
+      <c r="A24" s="30" t="s">
         <v>132</v>
       </c>
-      <c r="B24" s="28"/>
-      <c r="C24" s="28"/>
-      <c r="D24" s="28"/>
-      <c r="E24" s="28"/>
-      <c r="F24" s="28"/>
+      <c r="B24" s="31"/>
+      <c r="C24" s="31"/>
+      <c r="D24" s="31"/>
+      <c r="E24" s="31"/>
+      <c r="F24" s="31"/>
       <c r="G24" s="4"/>
       <c r="H24" s="4"/>
     </row>
     <row r="25" spans="1:8">
-      <c r="A25" s="20" t="s">
+      <c r="A25" s="30" t="s">
         <v>131</v>
       </c>
-      <c r="B25" s="28"/>
-      <c r="C25" s="28"/>
-      <c r="D25" s="28"/>
-      <c r="E25" s="28"/>
-      <c r="F25" s="28"/>
+      <c r="B25" s="31"/>
+      <c r="C25" s="31"/>
+      <c r="D25" s="31"/>
+      <c r="E25" s="31"/>
+      <c r="F25" s="31"/>
       <c r="G25" s="4"/>
       <c r="H25" s="4"/>
     </row>
@@ -2583,13 +2595,13 @@
       <c r="A26" s="5" t="s">
         <v>140</v>
       </c>
-      <c r="E26" s="33"/>
-      <c r="F26" s="33"/>
+      <c r="E26" s="29"/>
+      <c r="F26" s="29"/>
       <c r="G26" s="4"/>
       <c r="H26" s="4"/>
     </row>
     <row r="27" spans="1:8" ht="18.75">
-      <c r="A27" s="31" t="s">
+      <c r="A27" s="27" t="s">
         <v>141</v>
       </c>
       <c r="E27" s="16"/>
@@ -2598,25 +2610,25 @@
       <c r="H27" s="4"/>
     </row>
     <row r="28" spans="1:8" ht="15.75">
-      <c r="A28" s="29" t="s">
+      <c r="A28" s="25" t="s">
         <v>130</v>
       </c>
-      <c r="B28" s="29" t="s">
+      <c r="B28" s="25" t="s">
         <v>129</v>
       </c>
-      <c r="C28" s="29" t="s">
+      <c r="C28" s="25" t="s">
         <v>14</v>
       </c>
-      <c r="D28" s="30" t="s">
+      <c r="D28" s="26" t="s">
         <v>148</v>
       </c>
-      <c r="E28" s="30" t="s">
+      <c r="E28" s="26" t="s">
         <v>93</v>
       </c>
-      <c r="F28" s="30" t="s">
+      <c r="F28" s="26" t="s">
         <v>95</v>
       </c>
-      <c r="G28" s="32" t="s">
+      <c r="G28" s="28" t="s">
         <v>92</v>
       </c>
       <c r="H28" s="4"/>

</xml_diff>

<commit_message>
Some modification + add subscript "i"
</commit_message>
<xml_diff>
--- a/stm/documents/algorithm_and_tests/Short_Variable_List_Sediment_Version_02_10_11_version_2.xlsx
+++ b/stm/documents/algorithm_and_tests/Short_Variable_List_Sediment_Version_02_10_11_version_2.xlsx
@@ -102,9 +102,6 @@
     <t>Dimensionless particle number</t>
   </si>
   <si>
-    <t>D*</t>
-  </si>
-  <si>
     <t>q*</t>
   </si>
   <si>
@@ -220,9 +217,6 @@
     <t>Non-dimensional deposition function</t>
   </si>
   <si>
-    <t>Explicit Particle Reynolds number</t>
-  </si>
-  <si>
     <r>
       <t>τ</t>
     </r>
@@ -234,7 +228,67 @@
         <rFont val="Times New Roman"/>
         <family val="1"/>
       </rPr>
-      <t>bc</t>
+      <t>b</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>D</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>i</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>d</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>m</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>w</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>s</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>R</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>ep</t>
     </r>
   </si>
   <si>
@@ -249,12 +303,622 @@
         <rFont val="Times New Roman"/>
         <family val="1"/>
       </rPr>
+      <t>f</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Z</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>R</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>q</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
       <t>b</t>
     </r>
   </si>
   <si>
     <r>
-      <t>D</t>
+      <t>τ</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>bs</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>H</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">s </t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>H</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>f</t>
+    </r>
+  </si>
+  <si>
+    <t>Wetted Perimeter</t>
+  </si>
+  <si>
+    <t>Volume flow rate of suspended sediment per unit width</t>
+  </si>
+  <si>
+    <t>Volume flow rate of bed load per unit width</t>
+  </si>
+  <si>
+    <t>C</t>
+  </si>
+  <si>
+    <t>Sediment concentration in suspension</t>
+  </si>
+  <si>
+    <t>Particle Reynolds Number</t>
+  </si>
+  <si>
+    <r>
+      <t>Z</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>u</t>
+    </r>
+  </si>
+  <si>
+    <t>Garcia and Parker dimensionless shear stress</t>
+  </si>
+  <si>
+    <t>Reference concentration at the bottom</t>
+  </si>
+  <si>
+    <r>
+      <t>C</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>b</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>w</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>sc</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>τ</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>d, full</t>
+    </r>
+  </si>
+  <si>
+    <t>Critical shear stress for full deposition (Krone, 1962)</t>
+  </si>
+  <si>
+    <r>
+      <t>τ</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="superscript"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>c</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>s,e</t>
+    </r>
+  </si>
+  <si>
+    <t>Critical shear stress for surface erosion (Huang and Mehta, 1989)</t>
+  </si>
+  <si>
+    <r>
+      <t>ρ</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>s</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>ρ</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>b</t>
+    </r>
+  </si>
+  <si>
+    <t>Dry bulk density</t>
+  </si>
+  <si>
+    <r>
+      <t>LT</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="superscript"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>-2</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>L</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="superscript"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>2</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>T</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="superscript"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>-1</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>ML</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="superscript"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>-3</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>ρ</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>f</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>L</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="superscript"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>1/6</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>LT</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="superscript"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>-1</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>ML</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="superscript"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>-1</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>T</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="superscript"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>-2</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>L</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="superscript"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>2</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> T</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="superscript"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>-1</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve"> P</t>
+  </si>
+  <si>
+    <t>Constant</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Varies in </t>
+  </si>
+  <si>
+    <t>Parameters</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Space </t>
+  </si>
+  <si>
+    <t>State</t>
+  </si>
+  <si>
+    <t>B</t>
+  </si>
+  <si>
+    <t>Width</t>
+  </si>
+  <si>
+    <t>E, D</t>
+  </si>
+  <si>
+    <r>
+      <t>ν, D</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">i </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>, w</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">s </t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">u* </t>
+  </si>
+  <si>
+    <r>
+      <t>R</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">ep </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>, w</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>s</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>κ, w</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>s</t>
+    </r>
+  </si>
+  <si>
+    <t>Time and space</t>
+  </si>
+  <si>
+    <r>
+      <t>g , R</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>,ν , D</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">i </t>
+    </r>
+  </si>
+  <si>
+    <t>Constant (1)</t>
+  </si>
+  <si>
+    <t>Constant (2)</t>
+  </si>
+  <si>
+    <r>
+      <t>g , R ,ν , d</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>m</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+  </si>
+  <si>
+    <t>κ, n</t>
+  </si>
+  <si>
+    <t>ρ</t>
+  </si>
+  <si>
+    <r>
+      <t>g , R ,ν , D</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">i </t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">Constant </t>
+  </si>
+  <si>
+    <t>τ*</t>
+  </si>
+  <si>
+    <t>Shields parameter</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve"> R  , D</t>
     </r>
     <r>
       <rPr>
@@ -266,639 +930,8 @@
       </rPr>
       <t>i</t>
     </r>
-  </si>
-  <si>
-    <r>
-      <t>d</t>
-    </r>
-    <r>
-      <rPr>
-        <vertAlign val="subscript"/>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t>m</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>w</t>
-    </r>
-    <r>
-      <rPr>
-        <vertAlign val="subscript"/>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t>s</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>R</t>
-    </r>
-    <r>
-      <rPr>
-        <vertAlign val="subscript"/>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t>ep</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>R</t>
-    </r>
-    <r>
-      <rPr>
-        <vertAlign val="subscript"/>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t>f</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>τ</t>
-    </r>
-    <r>
-      <rPr>
-        <vertAlign val="subscript"/>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t>f</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>Z</t>
-    </r>
-    <r>
-      <rPr>
-        <vertAlign val="subscript"/>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t>R</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>q</t>
-    </r>
-    <r>
-      <rPr>
-        <vertAlign val="subscript"/>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t>b</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>τ</t>
-    </r>
-    <r>
-      <rPr>
-        <vertAlign val="subscript"/>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t>bs</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>H</t>
-    </r>
-    <r>
-      <rPr>
-        <vertAlign val="subscript"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t xml:space="preserve">s </t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>H</t>
-    </r>
-    <r>
-      <rPr>
-        <vertAlign val="subscript"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t>f</t>
-    </r>
-  </si>
-  <si>
-    <t>Wetted Perimeter</t>
-  </si>
-  <si>
-    <t>Volume flow rate of suspended sediment per unit width</t>
-  </si>
-  <si>
-    <t>Volume flow rate of bed load per unit width</t>
-  </si>
-  <si>
-    <t>C</t>
-  </si>
-  <si>
-    <t>Sediment concentration in suspension</t>
-  </si>
-  <si>
-    <t>Particle Reynolds Number</t>
-  </si>
-  <si>
-    <r>
-      <t>Z</t>
-    </r>
-    <r>
-      <rPr>
-        <vertAlign val="subscript"/>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t>u</t>
-    </r>
-  </si>
-  <si>
-    <t>Garcia and Parker dimensionless shear stress</t>
-  </si>
-  <si>
-    <t>Reference concentration at the bottom</t>
-  </si>
-  <si>
-    <r>
-      <t>C</t>
-    </r>
-    <r>
-      <rPr>
-        <vertAlign val="subscript"/>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t>b</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>w</t>
-    </r>
-    <r>
-      <rPr>
-        <vertAlign val="subscript"/>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t>sc</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>τ</t>
-    </r>
-    <r>
-      <rPr>
-        <vertAlign val="subscript"/>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t>d, full</t>
-    </r>
-  </si>
-  <si>
-    <t>Critical shear stress for full deposition (Krone, 1962)</t>
-  </si>
-  <si>
-    <r>
-      <t>τ</t>
-    </r>
-    <r>
-      <rPr>
-        <vertAlign val="superscript"/>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t>c</t>
-    </r>
-    <r>
-      <rPr>
-        <vertAlign val="subscript"/>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t>s,e</t>
-    </r>
-  </si>
-  <si>
-    <t>Critical shear stress for surface erosion (Huang and Mehta, 1989)</t>
-  </si>
-  <si>
-    <r>
-      <t>ρ</t>
-    </r>
-    <r>
-      <rPr>
-        <vertAlign val="subscript"/>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t>s</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>ρ</t>
-    </r>
-    <r>
-      <rPr>
-        <vertAlign val="subscript"/>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t>b</t>
-    </r>
-  </si>
-  <si>
-    <t>Dry bulk density</t>
-  </si>
-  <si>
-    <r>
-      <t>LT</t>
-    </r>
-    <r>
-      <rPr>
-        <vertAlign val="superscript"/>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t>-2</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>L</t>
-    </r>
-    <r>
-      <rPr>
-        <vertAlign val="superscript"/>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t>2</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t>T</t>
-    </r>
-    <r>
-      <rPr>
-        <vertAlign val="superscript"/>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t>-1</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>ML</t>
-    </r>
-    <r>
-      <rPr>
-        <vertAlign val="superscript"/>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t>-3</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>ρ</t>
-    </r>
-    <r>
-      <rPr>
-        <vertAlign val="subscript"/>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t>f</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>L</t>
-    </r>
-    <r>
-      <rPr>
-        <vertAlign val="superscript"/>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t>1/6</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>LT</t>
-    </r>
-    <r>
-      <rPr>
-        <vertAlign val="superscript"/>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t>-1</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>ML</t>
-    </r>
-    <r>
-      <rPr>
-        <vertAlign val="superscript"/>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t>-1</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t>T</t>
-    </r>
-    <r>
-      <rPr>
-        <vertAlign val="superscript"/>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t>-2</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>M L</t>
-    </r>
-    <r>
-      <rPr>
-        <vertAlign val="superscript"/>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t>-1</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t>T</t>
-    </r>
-    <r>
-      <rPr>
-        <vertAlign val="superscript"/>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t>-2</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>L</t>
-    </r>
-    <r>
-      <rPr>
-        <vertAlign val="superscript"/>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t>2</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t xml:space="preserve"> T</t>
-    </r>
-    <r>
-      <rPr>
-        <vertAlign val="superscript"/>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t>-1</t>
-    </r>
-  </si>
-  <si>
-    <t xml:space="preserve"> P</t>
-  </si>
-  <si>
-    <t>Constant</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Varies in </t>
-  </si>
-  <si>
-    <t>Parameters</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Space </t>
-  </si>
-  <si>
-    <t>State</t>
-  </si>
-  <si>
-    <t>B</t>
-  </si>
-  <si>
-    <t>Width</t>
-  </si>
-  <si>
-    <t>E, D</t>
-  </si>
-  <si>
-    <r>
-      <t>ν, D</t>
-    </r>
-    <r>
-      <rPr>
-        <vertAlign val="subscript"/>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t xml:space="preserve">i </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t>, w</t>
-    </r>
-    <r>
-      <rPr>
-        <vertAlign val="subscript"/>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t xml:space="preserve">s </t>
-    </r>
-  </si>
-  <si>
-    <t xml:space="preserve">u* </t>
-  </si>
-  <si>
-    <r>
-      <t>R</t>
-    </r>
-    <r>
-      <rPr>
-        <vertAlign val="subscript"/>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t xml:space="preserve">ep </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t>, w</t>
-    </r>
-    <r>
-      <rPr>
-        <vertAlign val="subscript"/>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t>s</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>κ, w</t>
-    </r>
-    <r>
-      <rPr>
-        <vertAlign val="subscript"/>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t>s</t>
-    </r>
-  </si>
-  <si>
-    <t>Time and space</t>
-  </si>
-  <si>
-    <r>
-      <t>g , R</t>
-    </r>
-    <r>
-      <rPr>
-        <vertAlign val="subscript"/>
+    <r>
+      <rPr>
         <sz val="11"/>
         <color rgb="FF000000"/>
         <rFont val="Times New Roman"/>
@@ -906,139 +939,9 @@
       </rPr>
       <t xml:space="preserve"> </t>
     </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t>,ν , D</t>
-    </r>
-    <r>
-      <rPr>
-        <vertAlign val="subscript"/>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t xml:space="preserve">i </t>
-    </r>
-  </si>
-  <si>
-    <t>Constant (1)</t>
-  </si>
-  <si>
-    <t>Constant (2)</t>
-  </si>
-  <si>
-    <r>
-      <t>g , R ,ν , d</t>
-    </r>
-    <r>
-      <rPr>
-        <vertAlign val="subscript"/>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t>m</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-  </si>
-  <si>
-    <t>κ, n</t>
-  </si>
-  <si>
-    <t>ρ</t>
-  </si>
-  <si>
-    <r>
-      <t>g , R ,ν , D</t>
-    </r>
-    <r>
-      <rPr>
-        <vertAlign val="subscript"/>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t xml:space="preserve">i </t>
-    </r>
-  </si>
-  <si>
-    <t xml:space="preserve">Constant </t>
-  </si>
-  <si>
-    <r>
-      <t>τ</t>
-    </r>
-    <r>
-      <rPr>
-        <vertAlign val="subscript"/>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t>c</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t>*</t>
-    </r>
-  </si>
-  <si>
-    <t>τ*</t>
-  </si>
-  <si>
-    <t>Shields parameter</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve"> R  , D</t>
-    </r>
-    <r>
-      <rPr>
-        <vertAlign val="subscript"/>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t>i</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
   </si>
   <si>
     <t>Critical Shields parameter</t>
-  </si>
-  <si>
-    <t>D*, φ</t>
   </si>
   <si>
     <r>
@@ -1215,9 +1118,6 @@
 This list is the result of the exchange of ideas during the meeting of 2/2/2011, and e-mail exchange during 2/11/2011. The current format of the table is suggested by Eli and Jamie on an email of 2/11/2011.</t>
   </si>
   <si>
-    <t>Time and space(3)</t>
-  </si>
-  <si>
     <t>Time and space (4)</t>
   </si>
   <si>
@@ -1236,7 +1136,119 @@
     </r>
   </si>
   <si>
-    <t xml:space="preserve">Wet Bulk density of the deposit </t>
+    <t>(3),(4) These are derived variable coming from HYDRO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Derived variable </t>
+  </si>
+  <si>
+    <r>
+      <t>w</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>si</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>g , R ,w</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>si</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> , Di </t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>w</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>si</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>D</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>i</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>/υ</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>K</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>s</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">B </t>
+  </si>
+  <si>
+    <t>U, H, u*</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Description </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sediment longitudinal dispersion coefficient </t>
   </si>
   <si>
     <r>
@@ -1250,79 +1262,27 @@
         <rFont val="Times New Roman"/>
         <family val="1"/>
       </rPr>
-      <t>d, particle</t>
-    </r>
-  </si>
-  <si>
-    <t xml:space="preserve">Critical shear stress for particle deposition </t>
-  </si>
-  <si>
-    <t>(3),(4) These are derived variable coming from HYDRO</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Derived variable </t>
-  </si>
-  <si>
-    <r>
-      <t>w</t>
-    </r>
-    <r>
-      <rPr>
-        <vertAlign val="subscript"/>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t>si</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>g , R ,w</t>
-    </r>
-    <r>
-      <rPr>
-        <vertAlign val="subscript"/>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t>si</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t xml:space="preserve"> , Di </t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>w</t>
-    </r>
-    <r>
-      <rPr>
-        <vertAlign val="subscript"/>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t>si</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t>D</t>
+      <t xml:space="preserve">bc, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>τ*</t>
+    </r>
+  </si>
+  <si>
+    <t>Fall (settling) velocity</t>
+  </si>
+  <si>
+    <t xml:space="preserve">U, H </t>
+  </si>
+  <si>
+    <r>
+      <t>H, D</t>
     </r>
     <r>
       <rPr>
@@ -1334,42 +1294,42 @@
       </rPr>
       <t>i</t>
     </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t>/υ</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>K</t>
-    </r>
-    <r>
-      <rPr>
-        <vertAlign val="subscript"/>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t>s</t>
-    </r>
-  </si>
-  <si>
-    <t xml:space="preserve">B </t>
-  </si>
-  <si>
-    <t>U, H, u*</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Description </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Sediment longitudinal dispersion coefficient </t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">R , </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>φ</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> , D</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>i</t>
+    </r>
+  </si>
+  <si>
+    <t>U, H, C</t>
   </si>
   <si>
     <r>
@@ -1383,27 +1343,69 @@
         <rFont val="Times New Roman"/>
         <family val="1"/>
       </rPr>
-      <t xml:space="preserve">bc, </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t>τ*</t>
-    </r>
-  </si>
-  <si>
-    <t>Fall (settling) velocity</t>
-  </si>
-  <si>
-    <t xml:space="preserve">U, H </t>
-  </si>
-  <si>
-    <r>
-      <t>H, D</t>
+      <t>d, partial</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">Wet bulk density of the deposit </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Critical shear stress for partial deposition </t>
+  </si>
+  <si>
+    <t>Time and space (3)</t>
+  </si>
+  <si>
+    <t>Explicit particle Reynolds number</t>
+  </si>
+  <si>
+    <r>
+      <t>R</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>epi</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>τ</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>bci</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>R</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>fi</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>D*</t>
     </r>
     <r>
       <rPr>
@@ -1418,25 +1420,50 @@
   </si>
   <si>
     <r>
-      <t xml:space="preserve">R , </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t>φ</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t xml:space="preserve"> , D</t>
+      <t>τ</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>ci</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>*</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>τ</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">bci </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>, g, R, ρ, D</t>
     </r>
     <r>
       <rPr>
@@ -1448,16 +1475,13 @@
       </rPr>
       <t>i</t>
     </r>
-  </si>
-  <si>
-    <t>U, H, C</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="15">
+  <fonts count="14">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1546,13 +1570,6 @@
       <family val="1"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Times New Roman"/>
-      <family val="1"/>
-    </font>
-    <font>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
       <name val="Times New Roman"/>
@@ -1802,7 +1819,6 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1816,6 +1832,9 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -1825,9 +1844,7 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2124,8 +2141,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:O56"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D18" sqref="D18"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="F38" sqref="F38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2144,7 +2161,7 @@
   <sheetData>
     <row r="1" spans="1:15" ht="15.75">
       <c r="B1" s="6" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C1" s="6"/>
       <c r="D1" s="6"/>
@@ -2162,7 +2179,7 @@
     </row>
     <row r="2" spans="1:15" ht="132.75" customHeight="1">
       <c r="B2" s="35" t="s">
-        <v>133</v>
+        <v>126</v>
       </c>
       <c r="C2" s="35"/>
       <c r="D2" s="35"/>
@@ -2180,7 +2197,7 @@
     </row>
     <row r="3" spans="1:15" ht="19.5" thickBot="1">
       <c r="A3" s="19" t="s">
-        <v>93</v>
+        <v>88</v>
       </c>
       <c r="B3" s="20"/>
       <c r="C3" s="20"/>
@@ -2188,7 +2205,7 @@
     </row>
     <row r="4" spans="1:15" ht="25.5">
       <c r="A4" s="21" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B4" s="22" t="s">
         <v>11</v>
@@ -2200,7 +2217,7 @@
         <v>15</v>
       </c>
       <c r="E4" s="23" t="s">
-        <v>92</v>
+        <v>87</v>
       </c>
       <c r="F4" s="15"/>
       <c r="G4" s="15"/>
@@ -2214,15 +2231,15 @@
         <v>16</v>
       </c>
       <c r="C5" s="11" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="D5" s="11" t="s">
         <v>0</v>
       </c>
       <c r="E5" s="10" t="s">
-        <v>91</v>
-      </c>
-      <c r="F5" s="30"/>
+        <v>86</v>
+      </c>
+      <c r="F5" s="29"/>
       <c r="G5" s="4"/>
       <c r="H5" s="4"/>
     </row>
@@ -2234,15 +2251,15 @@
         <v>17</v>
       </c>
       <c r="C6" s="11" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D6" s="11" t="s">
         <v>1</v>
       </c>
       <c r="E6" s="10" t="s">
-        <v>91</v>
-      </c>
-      <c r="F6" s="31"/>
+        <v>86</v>
+      </c>
+      <c r="F6" s="30"/>
       <c r="G6" s="4"/>
       <c r="H6" s="4"/>
     </row>
@@ -2254,15 +2271,15 @@
         <v>18</v>
       </c>
       <c r="C7" s="11" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="D7" s="11" t="s">
         <v>20</v>
       </c>
       <c r="E7" s="10" t="s">
-        <v>105</v>
-      </c>
-      <c r="F7" s="30"/>
+        <v>100</v>
+      </c>
+      <c r="F7" s="29"/>
       <c r="G7" s="4"/>
       <c r="H7" s="4"/>
     </row>
@@ -2274,15 +2291,15 @@
         <v>10</v>
       </c>
       <c r="C8" s="11" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="D8" s="11" t="s">
         <v>19</v>
       </c>
       <c r="E8" s="10" t="s">
-        <v>106</v>
-      </c>
-      <c r="F8" s="30"/>
+        <v>101</v>
+      </c>
+      <c r="F8" s="29"/>
       <c r="G8" s="4"/>
       <c r="H8" s="4"/>
     </row>
@@ -2291,18 +2308,18 @@
         <v>5</v>
       </c>
       <c r="B9" s="11" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="C9" s="11" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="D9" s="11" t="s">
         <v>4</v>
       </c>
       <c r="E9" s="10" t="s">
-        <v>91</v>
-      </c>
-      <c r="F9" s="30"/>
+        <v>86</v>
+      </c>
+      <c r="F9" s="29"/>
       <c r="G9" s="4"/>
       <c r="H9" s="4"/>
     </row>
@@ -2311,18 +2328,18 @@
         <v>6</v>
       </c>
       <c r="B10" s="11" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="C10" s="11" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="D10" s="11" t="s">
         <v>5</v>
       </c>
       <c r="E10" s="10" t="s">
-        <v>91</v>
-      </c>
-      <c r="F10" s="30"/>
+        <v>86</v>
+      </c>
+      <c r="F10" s="29"/>
       <c r="G10" s="4"/>
       <c r="H10" s="4"/>
     </row>
@@ -2331,7 +2348,7 @@
         <v>7</v>
       </c>
       <c r="B11" s="11" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="C11" s="11" t="s">
         <v>2</v>
@@ -2340,9 +2357,9 @@
         <v>7</v>
       </c>
       <c r="E11" s="10" t="s">
-        <v>91</v>
-      </c>
-      <c r="F11" s="30"/>
+        <v>86</v>
+      </c>
+      <c r="F11" s="29"/>
       <c r="G11" s="4"/>
       <c r="H11" s="4"/>
     </row>
@@ -2351,7 +2368,7 @@
         <v>8</v>
       </c>
       <c r="B12" s="11" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="C12" s="11" t="s">
         <v>2</v>
@@ -2360,9 +2377,9 @@
         <v>6</v>
       </c>
       <c r="E12" s="10" t="s">
-        <v>91</v>
-      </c>
-      <c r="F12" s="30"/>
+        <v>86</v>
+      </c>
+      <c r="F12" s="29"/>
       <c r="G12" s="4"/>
       <c r="H12" s="4"/>
     </row>
@@ -2371,18 +2388,18 @@
         <v>9</v>
       </c>
       <c r="B13" s="11" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="C13" s="7" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="D13" s="11" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="E13" s="8" t="s">
-        <v>91</v>
-      </c>
-      <c r="F13" s="30"/>
+        <v>86</v>
+      </c>
+      <c r="F13" s="29"/>
       <c r="G13" s="9"/>
       <c r="H13" s="9"/>
     </row>
@@ -2391,18 +2408,18 @@
         <v>10</v>
       </c>
       <c r="B14" s="11" t="s">
-        <v>136</v>
+        <v>128</v>
       </c>
       <c r="C14" s="11" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="D14" s="11" t="s">
-        <v>137</v>
+        <v>146</v>
       </c>
       <c r="E14" s="8" t="s">
-        <v>111</v>
-      </c>
-      <c r="F14" s="30"/>
+        <v>106</v>
+      </c>
+      <c r="F14" s="29"/>
       <c r="G14" s="9"/>
       <c r="H14" s="9"/>
     </row>
@@ -2411,18 +2428,18 @@
         <v>11</v>
       </c>
       <c r="B15" s="11" t="s">
-        <v>138</v>
+        <v>145</v>
       </c>
       <c r="C15" s="7" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="D15" s="11" t="s">
-        <v>139</v>
+        <v>147</v>
       </c>
       <c r="E15" s="8" t="s">
-        <v>111</v>
-      </c>
-      <c r="F15" s="30"/>
+        <v>106</v>
+      </c>
+      <c r="F15" s="29"/>
       <c r="G15" s="9"/>
       <c r="H15" s="9"/>
     </row>
@@ -2431,18 +2448,18 @@
         <v>12</v>
       </c>
       <c r="B16" s="11" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="C16" s="7" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="D16" s="11" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="E16" s="8" t="s">
-        <v>91</v>
-      </c>
-      <c r="F16" s="30"/>
+        <v>86</v>
+      </c>
+      <c r="F16" s="29"/>
       <c r="G16" s="9"/>
       <c r="H16" s="9"/>
     </row>
@@ -2451,18 +2468,18 @@
         <v>13</v>
       </c>
       <c r="B17" s="11" t="s">
+        <v>75</v>
+      </c>
+      <c r="C17" s="11" t="s">
         <v>79</v>
       </c>
-      <c r="C17" s="11" t="s">
-        <v>83</v>
-      </c>
       <c r="D17" s="11" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="E17" s="8" t="s">
-        <v>91</v>
-      </c>
-      <c r="F17" s="30"/>
+        <v>86</v>
+      </c>
+      <c r="F17" s="29"/>
       <c r="G17" s="9"/>
       <c r="H17" s="9"/>
     </row>
@@ -2471,18 +2488,18 @@
         <v>14</v>
       </c>
       <c r="B18" s="11" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="C18" s="11" t="s">
-        <v>88</v>
+        <v>83</v>
       </c>
       <c r="D18" s="11" t="s">
         <v>3</v>
       </c>
       <c r="E18" s="10" t="s">
-        <v>91</v>
-      </c>
-      <c r="F18" s="30"/>
+        <v>86</v>
+      </c>
+      <c r="F18" s="29"/>
       <c r="G18" s="4"/>
       <c r="H18" s="4"/>
     </row>
@@ -2491,18 +2508,18 @@
         <v>15</v>
       </c>
       <c r="B19" s="11" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
       <c r="C19" s="11" t="s">
         <v>2</v>
       </c>
       <c r="D19" s="11" t="s">
-        <v>97</v>
+        <v>92</v>
       </c>
       <c r="E19" s="10" t="s">
-        <v>94</v>
-      </c>
-      <c r="F19" s="36"/>
+        <v>89</v>
+      </c>
+      <c r="F19" s="32"/>
       <c r="G19" s="4"/>
       <c r="H19" s="4"/>
     </row>
@@ -2514,15 +2531,15 @@
         <v>8</v>
       </c>
       <c r="C20" s="11" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="D20" s="11" t="s">
         <v>9</v>
       </c>
       <c r="E20" s="10" t="s">
-        <v>94</v>
-      </c>
-      <c r="F20" s="36"/>
+        <v>89</v>
+      </c>
+      <c r="F20" s="32"/>
       <c r="G20" s="4"/>
       <c r="H20" s="4"/>
     </row>
@@ -2534,15 +2551,15 @@
         <v>12</v>
       </c>
       <c r="C21" s="11" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="D21" s="11" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E21" s="10" t="s">
-        <v>134</v>
-      </c>
-      <c r="F21" s="32"/>
+        <v>148</v>
+      </c>
+      <c r="F21" s="31"/>
       <c r="G21" s="4"/>
       <c r="H21" s="4"/>
     </row>
@@ -2557,12 +2574,12 @@
         <v>2</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E22" s="14" t="s">
-        <v>135</v>
-      </c>
-      <c r="F22" s="32"/>
+        <v>127</v>
+      </c>
+      <c r="F22" s="31"/>
       <c r="G22" s="4"/>
       <c r="H22" s="4"/>
     </row>
@@ -2578,7 +2595,7 @@
     </row>
     <row r="24" spans="1:8">
       <c r="A24" s="33" t="s">
-        <v>132</v>
+        <v>125</v>
       </c>
       <c r="B24" s="34"/>
       <c r="C24" s="34"/>
@@ -2590,7 +2607,7 @@
     </row>
     <row r="25" spans="1:8">
       <c r="A25" s="33" t="s">
-        <v>131</v>
+        <v>124</v>
       </c>
       <c r="B25" s="34"/>
       <c r="C25" s="34"/>
@@ -2602,16 +2619,16 @@
     </row>
     <row r="26" spans="1:8">
       <c r="A26" s="5" t="s">
-        <v>140</v>
-      </c>
-      <c r="E26" s="29"/>
-      <c r="F26" s="29"/>
+        <v>129</v>
+      </c>
+      <c r="E26" s="28"/>
+      <c r="F26" s="28"/>
       <c r="G26" s="4"/>
       <c r="H26" s="4"/>
     </row>
     <row r="27" spans="1:8" ht="18.75">
-      <c r="A27" s="27" t="s">
-        <v>141</v>
+      <c r="A27" s="36" t="s">
+        <v>130</v>
       </c>
       <c r="E27" s="16"/>
       <c r="F27" s="16"/>
@@ -2620,25 +2637,25 @@
     </row>
     <row r="28" spans="1:8" ht="15.75">
       <c r="A28" s="25" t="s">
-        <v>130</v>
+        <v>123</v>
       </c>
       <c r="B28" s="25" t="s">
-        <v>129</v>
+        <v>122</v>
       </c>
       <c r="C28" s="25" t="s">
         <v>14</v>
       </c>
       <c r="D28" s="26" t="s">
-        <v>148</v>
+        <v>137</v>
       </c>
       <c r="E28" s="26" t="s">
-        <v>93</v>
+        <v>88</v>
       </c>
       <c r="F28" s="26" t="s">
-        <v>95</v>
-      </c>
-      <c r="G28" s="28" t="s">
-        <v>92</v>
+        <v>90</v>
+      </c>
+      <c r="G28" s="27" t="s">
+        <v>87</v>
       </c>
       <c r="H28" s="4"/>
     </row>
@@ -2650,19 +2667,19 @@
         <v>25</v>
       </c>
       <c r="C29" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="D29" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="D29" s="7" t="s">
-        <v>34</v>
-      </c>
       <c r="E29" s="11" t="s">
-        <v>121</v>
+        <v>114</v>
       </c>
       <c r="F29" s="11" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
       <c r="G29" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="H29" s="9"/>
     </row>
@@ -2671,22 +2688,22 @@
         <v>20</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>142</v>
+        <v>131</v>
       </c>
       <c r="C30" s="7" t="s">
+        <v>82</v>
+      </c>
+      <c r="D30" s="7" t="s">
+        <v>140</v>
+      </c>
+      <c r="E30" s="11" t="s">
+        <v>99</v>
+      </c>
+      <c r="F30" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="D30" s="7" t="s">
-        <v>151</v>
-      </c>
-      <c r="E30" s="11" t="s">
-        <v>104</v>
-      </c>
-      <c r="F30" s="1" t="s">
-        <v>91</v>
-      </c>
       <c r="G30" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="H30" s="9"/>
     </row>
@@ -2695,22 +2712,22 @@
         <v>21</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>55</v>
+        <v>150</v>
       </c>
       <c r="C31" s="7" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D31" s="7" t="s">
-        <v>49</v>
+        <v>149</v>
       </c>
       <c r="E31" s="11" t="s">
-        <v>143</v>
+        <v>132</v>
       </c>
       <c r="F31" s="11" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
       <c r="G31" s="11" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="H31" s="4"/>
     </row>
@@ -2719,22 +2736,22 @@
         <v>22</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>50</v>
+        <v>151</v>
       </c>
       <c r="C32" s="7" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="D32" s="7" t="s">
         <v>23</v>
       </c>
       <c r="E32" s="11" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="F32" s="11" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
       <c r="G32" s="11" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="H32" s="4"/>
     </row>
@@ -2743,22 +2760,22 @@
         <v>23</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>56</v>
+        <v>152</v>
       </c>
       <c r="C33" s="7" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D33" s="7" t="s">
         <v>24</v>
       </c>
       <c r="E33" s="11" t="s">
-        <v>110</v>
+        <v>105</v>
       </c>
       <c r="F33" s="11" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
       <c r="G33" s="11" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="H33" s="4"/>
     </row>
@@ -2767,22 +2784,22 @@
         <v>24</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>28</v>
+        <v>153</v>
       </c>
       <c r="C34" s="7" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D34" s="7" t="s">
         <v>27</v>
       </c>
       <c r="E34" s="11" t="s">
-        <v>110</v>
+        <v>105</v>
       </c>
       <c r="F34" s="11" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
       <c r="G34" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="H34" s="9"/>
     </row>
@@ -2791,22 +2808,22 @@
         <v>25</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>112</v>
+        <v>154</v>
       </c>
       <c r="C35" s="7" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D35" s="7" t="s">
-        <v>116</v>
+        <v>110</v>
       </c>
       <c r="E35" s="11" t="s">
-        <v>117</v>
+        <v>155</v>
       </c>
       <c r="F35" s="11" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
       <c r="G35" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="H35" s="9"/>
     </row>
@@ -2815,22 +2832,22 @@
         <v>26</v>
       </c>
       <c r="B36" s="11" t="s">
-        <v>144</v>
+        <v>133</v>
       </c>
       <c r="C36" s="11" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D36" s="11" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="E36" s="1" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="F36" s="1" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
       <c r="G36" s="11" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="H36" s="4"/>
     </row>
@@ -2839,22 +2856,22 @@
         <v>27</v>
       </c>
       <c r="B37" s="11" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="C37" s="11" t="s">
+        <v>82</v>
+      </c>
+      <c r="D37" s="11" t="s">
+        <v>116</v>
+      </c>
+      <c r="E37" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="F37" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="D37" s="11" t="s">
-        <v>123</v>
-      </c>
-      <c r="E37" s="1" t="s">
-        <v>107</v>
-      </c>
-      <c r="F37" s="1" t="s">
-        <v>91</v>
-      </c>
       <c r="G37" s="11" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="H37" s="4"/>
     </row>
@@ -2863,22 +2880,22 @@
         <v>28</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C38" s="7" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="D38" s="7" t="s">
         <v>21</v>
       </c>
       <c r="E38" s="1" t="s">
-        <v>108</v>
+        <v>103</v>
       </c>
       <c r="F38" s="1" t="s">
-        <v>152</v>
+        <v>141</v>
       </c>
       <c r="G38" s="1" t="s">
-        <v>103</v>
+        <v>98</v>
       </c>
       <c r="H38" s="9"/>
     </row>
@@ -2887,22 +2904,22 @@
         <v>29</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="C39" s="7" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="D39" s="7" t="s">
         <v>22</v>
       </c>
       <c r="E39" s="1" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
       <c r="F39" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="G39" s="1" t="s">
-        <v>103</v>
+        <v>98</v>
       </c>
       <c r="H39" s="9"/>
     </row>
@@ -2911,22 +2928,22 @@
         <v>30</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>113</v>
+        <v>107</v>
       </c>
       <c r="C40" s="7" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D40" s="7" t="s">
-        <v>114</v>
+        <v>108</v>
       </c>
       <c r="E40" s="11" t="s">
-        <v>115</v>
+        <v>109</v>
       </c>
       <c r="F40" s="1" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="G40" s="1" t="s">
-        <v>103</v>
+        <v>98</v>
       </c>
       <c r="H40" s="9"/>
     </row>
@@ -2935,22 +2952,22 @@
         <v>31</v>
       </c>
       <c r="B41" s="11" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="C41" s="11" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D41" s="11" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E41" s="1" t="s">
-        <v>102</v>
+        <v>97</v>
       </c>
       <c r="F41" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="G41" s="1" t="s">
-        <v>103</v>
+        <v>98</v>
       </c>
       <c r="H41" s="9"/>
     </row>
@@ -2959,22 +2976,22 @@
         <v>32</v>
       </c>
       <c r="B42" s="11" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="C42" s="7" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D42" s="11" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="E42" s="1" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="F42" s="1" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="G42" s="1" t="s">
-        <v>103</v>
+        <v>98</v>
       </c>
       <c r="H42" s="9"/>
     </row>
@@ -2983,22 +3000,22 @@
         <v>33</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C43" s="7" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="D43" s="7" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E43" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="F43" s="1" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="G43" s="1" t="s">
-        <v>103</v>
+        <v>98</v>
       </c>
       <c r="H43" s="9"/>
     </row>
@@ -3007,22 +3024,22 @@
         <v>34</v>
       </c>
       <c r="B44" s="11" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="C44" s="11" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D44" s="11" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="E44" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="F44" s="1" t="s">
-        <v>150</v>
+        <v>139</v>
       </c>
       <c r="G44" s="1" t="s">
-        <v>103</v>
+        <v>98</v>
       </c>
       <c r="H44" s="9"/>
     </row>
@@ -3031,22 +3048,22 @@
         <v>35</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C45" s="7" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="D45" s="7" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E45" s="1" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="F45" s="1" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="G45" s="1" t="s">
-        <v>103</v>
+        <v>98</v>
       </c>
       <c r="H45" s="4"/>
     </row>
@@ -3055,22 +3072,22 @@
         <v>36</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>145</v>
+        <v>134</v>
       </c>
       <c r="C46" s="7" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
       <c r="D46" s="7" t="s">
-        <v>149</v>
+        <v>138</v>
       </c>
       <c r="E46" s="1" t="s">
-        <v>146</v>
+        <v>135</v>
       </c>
       <c r="F46" s="1" t="s">
-        <v>147</v>
+        <v>136</v>
       </c>
       <c r="G46" s="1" t="s">
-        <v>103</v>
+        <v>98</v>
       </c>
       <c r="H46" s="4"/>
     </row>
@@ -3079,22 +3096,22 @@
         <v>37</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C47" s="7" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D47" s="7" t="s">
         <v>26</v>
       </c>
       <c r="E47" s="1" t="s">
-        <v>154</v>
+        <v>143</v>
       </c>
       <c r="F47" s="1" t="s">
-        <v>118</v>
+        <v>111</v>
       </c>
       <c r="G47" s="1" t="s">
-        <v>103</v>
+        <v>98</v>
       </c>
       <c r="H47" s="9"/>
     </row>
@@ -3103,22 +3120,22 @@
         <v>38</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>127</v>
+        <v>120</v>
       </c>
       <c r="C48" s="7" t="s">
         <v>2</v>
       </c>
       <c r="D48" s="7" t="s">
-        <v>128</v>
+        <v>121</v>
       </c>
       <c r="E48" s="11" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="F48" s="11" t="s">
-        <v>153</v>
+        <v>142</v>
       </c>
       <c r="G48" s="1" t="s">
-        <v>103</v>
+        <v>98</v>
       </c>
       <c r="H48" s="4"/>
     </row>
@@ -3127,22 +3144,22 @@
         <v>39</v>
       </c>
       <c r="B49" s="11" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="C49" s="11" t="s">
         <v>2</v>
       </c>
       <c r="D49" s="11" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="E49" s="11" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="F49" s="11" t="s">
         <v>13</v>
       </c>
       <c r="G49" s="1" t="s">
-        <v>103</v>
+        <v>98</v>
       </c>
       <c r="H49" s="9"/>
     </row>
@@ -3151,22 +3168,22 @@
         <v>40</v>
       </c>
       <c r="B50" s="11" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C50" s="11" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
       <c r="D50" s="11" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="E50" s="1" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="F50" s="1" t="s">
-        <v>155</v>
+        <v>144</v>
       </c>
       <c r="G50" s="1" t="s">
-        <v>103</v>
+        <v>98</v>
       </c>
       <c r="H50" s="4"/>
     </row>
@@ -3175,22 +3192,22 @@
         <v>41</v>
       </c>
       <c r="B51" s="17" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="C51" s="17" t="s">
         <v>2</v>
       </c>
       <c r="D51" s="17" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E51" s="18" t="s">
-        <v>125</v>
+        <v>118</v>
       </c>
       <c r="F51" s="18" t="s">
-        <v>126</v>
+        <v>119</v>
       </c>
       <c r="G51" s="1" t="s">
-        <v>103</v>
+        <v>98</v>
       </c>
       <c r="H51" s="9"/>
     </row>
@@ -3199,22 +3216,22 @@
         <v>42</v>
       </c>
       <c r="B52" s="17" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="C52" s="17" t="s">
         <v>2</v>
       </c>
       <c r="D52" s="17" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E52" s="18" t="s">
-        <v>125</v>
+        <v>118</v>
       </c>
       <c r="F52" s="18" t="s">
-        <v>124</v>
+        <v>117</v>
       </c>
       <c r="G52" s="1" t="s">
-        <v>103</v>
+        <v>98</v>
       </c>
       <c r="H52" s="9"/>
     </row>
@@ -3223,22 +3240,22 @@
         <v>43</v>
       </c>
       <c r="B53" s="11" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="C53" s="11" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D53" s="11" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="E53" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="F53" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="G53" s="1" t="s">
         <v>98</v>
-      </c>
-      <c r="G53" s="1" t="s">
-        <v>103</v>
       </c>
       <c r="H53" s="9"/>
     </row>
@@ -3247,22 +3264,22 @@
         <v>44</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C54" s="7" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="D54" s="3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E54" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="F54" s="1" t="s">
-        <v>119</v>
+        <v>112</v>
       </c>
       <c r="G54" s="1" t="s">
-        <v>103</v>
+        <v>98</v>
       </c>
       <c r="H54" s="9"/>
     </row>
@@ -3271,22 +3288,22 @@
         <v>45</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="C55" s="7" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="D55" s="3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E55" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="F55" s="1" t="s">
-        <v>120</v>
+        <v>113</v>
       </c>
       <c r="G55" s="1" t="s">
-        <v>103</v>
+        <v>98</v>
       </c>
       <c r="H55" s="4"/>
     </row>
@@ -3295,22 +3312,22 @@
         <v>46</v>
       </c>
       <c r="B56" s="11" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="C56" s="11" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
       <c r="D56" s="11" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="E56" s="1" t="s">
-        <v>122</v>
+        <v>115</v>
       </c>
       <c r="F56" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="G56" s="1" t="s">
-        <v>103</v>
+        <v>98</v>
       </c>
       <c r="H56" s="9"/>
     </row>

</xml_diff>

<commit_message>
Modification on the angle of repose and Hs and Hf
</commit_message>
<xml_diff>
--- a/stm/documents/algorithm_and_tests/Short_Variable_List_Sediment_Version_02_10_11_version_2.xlsx
+++ b/stm/documents/algorithm_and_tests/Short_Variable_List_Sediment_Version_02_10_11_version_2.xlsx
@@ -863,30 +863,6 @@
     <t>Constant (2)</t>
   </si>
   <si>
-    <r>
-      <t>g , R ,ν , d</t>
-    </r>
-    <r>
-      <rPr>
-        <vertAlign val="subscript"/>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t>m</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-  </si>
-  <si>
     <t>κ, n</t>
   </si>
   <si>
@@ -917,8 +893,50 @@
     <t>Shields parameter</t>
   </si>
   <si>
-    <r>
-      <t xml:space="preserve"> R  , D</t>
+    <t>Critical Shields parameter</t>
+  </si>
+  <si>
+    <r>
+      <t>τ</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>c</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>*,τ*</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>ρ, ρ</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>s</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>g , R , D</t>
     </r>
     <r>
       <rPr>
@@ -930,138 +948,9 @@
       </rPr>
       <t>i</t>
     </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-  </si>
-  <si>
-    <t>Critical Shields parameter</t>
-  </si>
-  <si>
-    <r>
-      <t>τ</t>
-    </r>
-    <r>
-      <rPr>
-        <vertAlign val="subscript"/>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t>c</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t>*,τ*</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>H</t>
-    </r>
-    <r>
-      <rPr>
-        <vertAlign val="subscript"/>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t>f</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>H</t>
-    </r>
-    <r>
-      <rPr>
-        <vertAlign val="subscript"/>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t>s</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>ρ, ρ</t>
-    </r>
-    <r>
-      <rPr>
-        <vertAlign val="subscript"/>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t>s</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>g , R , D</t>
-    </r>
-    <r>
-      <rPr>
-        <vertAlign val="subscript"/>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t>i</t>
-    </r>
   </si>
   <si>
     <t>Cohesive sediment settling velocity</t>
-  </si>
-  <si>
-    <t>H, U</t>
-  </si>
-  <si>
-    <r>
-      <t>Bed Slope, κ, K</t>
-    </r>
-    <r>
-      <rPr>
-        <vertAlign val="subscript"/>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t>s</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>H, H</t>
-    </r>
-    <r>
-      <rPr>
-        <vertAlign val="subscript"/>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t>s</t>
-    </r>
   </si>
   <si>
     <t>b</t>
@@ -1296,26 +1185,83 @@
     </r>
   </si>
   <si>
-    <r>
-      <t xml:space="preserve">R , </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t>φ</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t xml:space="preserve"> , D</t>
+    <t>U, H, C</t>
+  </si>
+  <si>
+    <r>
+      <t>τ</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>d, partial</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">Wet bulk density of the deposit </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Critical shear stress for partial deposition </t>
+  </si>
+  <si>
+    <t>Time and space (3)</t>
+  </si>
+  <si>
+    <t>Explicit particle Reynolds number</t>
+  </si>
+  <si>
+    <r>
+      <t>R</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>epi</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>τ</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>bci</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>R</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>fi</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>D*</t>
     </r>
     <r>
       <rPr>
@@ -1329,9 +1275,6 @@
     </r>
   </si>
   <si>
-    <t>U, H, C</t>
-  </si>
-  <si>
     <r>
       <t>τ</t>
     </r>
@@ -1343,34 +1286,16 @@
         <rFont val="Times New Roman"/>
         <family val="1"/>
       </rPr>
-      <t>d, partial</t>
-    </r>
-  </si>
-  <si>
-    <t xml:space="preserve">Wet bulk density of the deposit </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Critical shear stress for partial deposition </t>
-  </si>
-  <si>
-    <t>Time and space (3)</t>
-  </si>
-  <si>
-    <t>Explicit particle Reynolds number</t>
-  </si>
-  <si>
-    <r>
-      <t>R</t>
-    </r>
-    <r>
-      <rPr>
-        <vertAlign val="subscript"/>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t>epi</t>
+      <t>ci</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>*</t>
     </r>
   </si>
   <si>
@@ -1385,27 +1310,16 @@
         <rFont val="Times New Roman"/>
         <family val="1"/>
       </rPr>
-      <t>bci</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>R</t>
-    </r>
-    <r>
-      <rPr>
-        <vertAlign val="subscript"/>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t>fi</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>D*</t>
+      <t xml:space="preserve">bci </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>, g, R, ρ, D</t>
     </r>
     <r>
       <rPr>
@@ -1420,50 +1334,31 @@
   </si>
   <si>
     <r>
-      <t>τ</t>
-    </r>
-    <r>
-      <rPr>
-        <vertAlign val="subscript"/>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t>ci</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t>*</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>τ</t>
-    </r>
-    <r>
-      <rPr>
-        <vertAlign val="subscript"/>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t xml:space="preserve">bci </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t>, g, R, ρ, D</t>
+      <t>g , R, ν, d</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>m</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>g, R, D</t>
     </r>
     <r>
       <rPr>
@@ -1474,6 +1369,102 @@
         <family val="1"/>
       </rPr>
       <t>i</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>R,</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> D</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>i</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve"> κ, K</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>s</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>u*, H, H</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>s</t>
+    </r>
+  </si>
+  <si>
+    <t>H, u*</t>
+  </si>
+  <si>
+    <r>
+      <t>u*, H</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>f</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>u*, H</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>s</t>
     </r>
   </si>
 </sst>
@@ -1481,7 +1472,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="14">
+  <fonts count="13">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1569,12 +1560,6 @@
       <name val="Times New Roman"/>
       <family val="1"/>
     </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Times New Roman"/>
-      <family val="1"/>
-    </font>
   </fonts>
   <fills count="5">
     <fill>
@@ -1795,12 +1780,6 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1835,6 +1814,7 @@
     <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -1844,7 +1824,12 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2141,8 +2126,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:O56"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="F38" sqref="F38"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="G61" sqref="G61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2178,45 +2163,45 @@
       <c r="O1" s="6"/>
     </row>
     <row r="2" spans="1:15" ht="132.75" customHeight="1">
-      <c r="B2" s="35" t="s">
-        <v>126</v>
-      </c>
-      <c r="C2" s="35"/>
-      <c r="D2" s="35"/>
-      <c r="E2" s="35"/>
-      <c r="F2" s="35"/>
-      <c r="G2" s="35"/>
-      <c r="H2" s="35"/>
-      <c r="I2" s="35"/>
-      <c r="J2" s="35"/>
-      <c r="K2" s="35"/>
-      <c r="L2" s="35"/>
-      <c r="M2" s="35"/>
-      <c r="N2" s="35"/>
-      <c r="O2" s="35"/>
+      <c r="B2" s="34" t="s">
+        <v>119</v>
+      </c>
+      <c r="C2" s="34"/>
+      <c r="D2" s="34"/>
+      <c r="E2" s="34"/>
+      <c r="F2" s="34"/>
+      <c r="G2" s="34"/>
+      <c r="H2" s="34"/>
+      <c r="I2" s="34"/>
+      <c r="J2" s="34"/>
+      <c r="K2" s="34"/>
+      <c r="L2" s="34"/>
+      <c r="M2" s="34"/>
+      <c r="N2" s="34"/>
+      <c r="O2" s="34"/>
     </row>
     <row r="3" spans="1:15" ht="19.5" thickBot="1">
-      <c r="A3" s="19" t="s">
+      <c r="A3" s="17" t="s">
         <v>88</v>
       </c>
-      <c r="B3" s="20"/>
-      <c r="C3" s="20"/>
-      <c r="D3" s="20"/>
+      <c r="B3" s="18"/>
+      <c r="C3" s="18"/>
+      <c r="D3" s="18"/>
     </row>
     <row r="4" spans="1:15" ht="25.5">
-      <c r="A4" s="21" t="s">
+      <c r="A4" s="19" t="s">
         <v>37</v>
       </c>
-      <c r="B4" s="22" t="s">
+      <c r="B4" s="20" t="s">
         <v>11</v>
       </c>
-      <c r="C4" s="22" t="s">
+      <c r="C4" s="20" t="s">
         <v>14</v>
       </c>
-      <c r="D4" s="22" t="s">
+      <c r="D4" s="20" t="s">
         <v>15</v>
       </c>
-      <c r="E4" s="23" t="s">
+      <c r="E4" s="21" t="s">
         <v>87</v>
       </c>
       <c r="F4" s="15"/>
@@ -2239,7 +2224,7 @@
       <c r="E5" s="10" t="s">
         <v>86</v>
       </c>
-      <c r="F5" s="29"/>
+      <c r="F5" s="27"/>
       <c r="G5" s="4"/>
       <c r="H5" s="4"/>
     </row>
@@ -2259,7 +2244,7 @@
       <c r="E6" s="10" t="s">
         <v>86</v>
       </c>
-      <c r="F6" s="30"/>
+      <c r="F6" s="28"/>
       <c r="G6" s="4"/>
       <c r="H6" s="4"/>
     </row>
@@ -2279,7 +2264,7 @@
       <c r="E7" s="10" t="s">
         <v>100</v>
       </c>
-      <c r="F7" s="29"/>
+      <c r="F7" s="27"/>
       <c r="G7" s="4"/>
       <c r="H7" s="4"/>
     </row>
@@ -2299,7 +2284,7 @@
       <c r="E8" s="10" t="s">
         <v>101</v>
       </c>
-      <c r="F8" s="29"/>
+      <c r="F8" s="27"/>
       <c r="G8" s="4"/>
       <c r="H8" s="4"/>
     </row>
@@ -2319,7 +2304,7 @@
       <c r="E9" s="10" t="s">
         <v>86</v>
       </c>
-      <c r="F9" s="29"/>
+      <c r="F9" s="27"/>
       <c r="G9" s="4"/>
       <c r="H9" s="4"/>
     </row>
@@ -2339,7 +2324,7 @@
       <c r="E10" s="10" t="s">
         <v>86</v>
       </c>
-      <c r="F10" s="29"/>
+      <c r="F10" s="27"/>
       <c r="G10" s="4"/>
       <c r="H10" s="4"/>
     </row>
@@ -2359,7 +2344,7 @@
       <c r="E11" s="10" t="s">
         <v>86</v>
       </c>
-      <c r="F11" s="29"/>
+      <c r="F11" s="27"/>
       <c r="G11" s="4"/>
       <c r="H11" s="4"/>
     </row>
@@ -2379,7 +2364,7 @@
       <c r="E12" s="10" t="s">
         <v>86</v>
       </c>
-      <c r="F12" s="29"/>
+      <c r="F12" s="27"/>
       <c r="G12" s="4"/>
       <c r="H12" s="4"/>
     </row>
@@ -2399,7 +2384,7 @@
       <c r="E13" s="8" t="s">
         <v>86</v>
       </c>
-      <c r="F13" s="29"/>
+      <c r="F13" s="27"/>
       <c r="G13" s="9"/>
       <c r="H13" s="9"/>
     </row>
@@ -2408,18 +2393,18 @@
         <v>10</v>
       </c>
       <c r="B14" s="11" t="s">
-        <v>128</v>
+        <v>121</v>
       </c>
       <c r="C14" s="11" t="s">
         <v>79</v>
       </c>
       <c r="D14" s="11" t="s">
-        <v>146</v>
+        <v>138</v>
       </c>
       <c r="E14" s="8" t="s">
-        <v>106</v>
-      </c>
-      <c r="F14" s="29"/>
+        <v>105</v>
+      </c>
+      <c r="F14" s="27"/>
       <c r="G14" s="9"/>
       <c r="H14" s="9"/>
     </row>
@@ -2428,18 +2413,18 @@
         <v>11</v>
       </c>
       <c r="B15" s="11" t="s">
-        <v>145</v>
+        <v>137</v>
       </c>
       <c r="C15" s="7" t="s">
         <v>83</v>
       </c>
       <c r="D15" s="11" t="s">
-        <v>147</v>
+        <v>139</v>
       </c>
       <c r="E15" s="8" t="s">
-        <v>106</v>
-      </c>
-      <c r="F15" s="29"/>
+        <v>105</v>
+      </c>
+      <c r="F15" s="27"/>
       <c r="G15" s="9"/>
       <c r="H15" s="9"/>
     </row>
@@ -2459,7 +2444,7 @@
       <c r="E16" s="8" t="s">
         <v>86</v>
       </c>
-      <c r="F16" s="29"/>
+      <c r="F16" s="27"/>
       <c r="G16" s="9"/>
       <c r="H16" s="9"/>
     </row>
@@ -2479,7 +2464,7 @@
       <c r="E17" s="8" t="s">
         <v>86</v>
       </c>
-      <c r="F17" s="29"/>
+      <c r="F17" s="27"/>
       <c r="G17" s="9"/>
       <c r="H17" s="9"/>
     </row>
@@ -2499,7 +2484,7 @@
       <c r="E18" s="10" t="s">
         <v>86</v>
       </c>
-      <c r="F18" s="29"/>
+      <c r="F18" s="27"/>
       <c r="G18" s="4"/>
       <c r="H18" s="4"/>
     </row>
@@ -2519,7 +2504,7 @@
       <c r="E19" s="10" t="s">
         <v>89</v>
       </c>
-      <c r="F19" s="32"/>
+      <c r="F19" s="30"/>
       <c r="G19" s="4"/>
       <c r="H19" s="4"/>
     </row>
@@ -2539,7 +2524,7 @@
       <c r="E20" s="10" t="s">
         <v>89</v>
       </c>
-      <c r="F20" s="32"/>
+      <c r="F20" s="30"/>
       <c r="G20" s="4"/>
       <c r="H20" s="4"/>
     </row>
@@ -2557,14 +2542,14 @@
         <v>41</v>
       </c>
       <c r="E21" s="10" t="s">
-        <v>148</v>
-      </c>
-      <c r="F21" s="31"/>
+        <v>140</v>
+      </c>
+      <c r="F21" s="29"/>
       <c r="G21" s="4"/>
       <c r="H21" s="4"/>
     </row>
     <row r="22" spans="1:8" ht="15.75" thickBot="1">
-      <c r="A22" s="24">
+      <c r="A22" s="22">
         <v>18</v>
       </c>
       <c r="B22" s="2" t="s">
@@ -2577,9 +2562,9 @@
         <v>42</v>
       </c>
       <c r="E22" s="14" t="s">
-        <v>127</v>
-      </c>
-      <c r="F22" s="31"/>
+        <v>120</v>
+      </c>
+      <c r="F22" s="29"/>
       <c r="G22" s="4"/>
       <c r="H22" s="4"/>
     </row>
@@ -2594,41 +2579,41 @@
       <c r="H23" s="4"/>
     </row>
     <row r="24" spans="1:8">
-      <c r="A24" s="33" t="s">
-        <v>125</v>
-      </c>
-      <c r="B24" s="34"/>
-      <c r="C24" s="34"/>
-      <c r="D24" s="34"/>
-      <c r="E24" s="34"/>
-      <c r="F24" s="34"/>
+      <c r="A24" s="32" t="s">
+        <v>118</v>
+      </c>
+      <c r="B24" s="33"/>
+      <c r="C24" s="33"/>
+      <c r="D24" s="33"/>
+      <c r="E24" s="33"/>
+      <c r="F24" s="33"/>
       <c r="G24" s="4"/>
       <c r="H24" s="4"/>
     </row>
     <row r="25" spans="1:8">
-      <c r="A25" s="33" t="s">
-        <v>124</v>
-      </c>
-      <c r="B25" s="34"/>
-      <c r="C25" s="34"/>
-      <c r="D25" s="34"/>
-      <c r="E25" s="34"/>
-      <c r="F25" s="34"/>
+      <c r="A25" s="32" t="s">
+        <v>117</v>
+      </c>
+      <c r="B25" s="33"/>
+      <c r="C25" s="33"/>
+      <c r="D25" s="33"/>
+      <c r="E25" s="33"/>
+      <c r="F25" s="33"/>
       <c r="G25" s="4"/>
       <c r="H25" s="4"/>
     </row>
     <row r="26" spans="1:8">
       <c r="A26" s="5" t="s">
-        <v>129</v>
-      </c>
-      <c r="E26" s="28"/>
-      <c r="F26" s="28"/>
+        <v>122</v>
+      </c>
+      <c r="E26" s="26"/>
+      <c r="F26" s="26"/>
       <c r="G26" s="4"/>
       <c r="H26" s="4"/>
     </row>
     <row r="27" spans="1:8" ht="18.75">
-      <c r="A27" s="36" t="s">
-        <v>130</v>
+      <c r="A27" s="31" t="s">
+        <v>123</v>
       </c>
       <c r="E27" s="16"/>
       <c r="F27" s="16"/>
@@ -2636,25 +2621,25 @@
       <c r="H27" s="4"/>
     </row>
     <row r="28" spans="1:8" ht="15.75">
-      <c r="A28" s="25" t="s">
-        <v>123</v>
-      </c>
-      <c r="B28" s="25" t="s">
-        <v>122</v>
-      </c>
-      <c r="C28" s="25" t="s">
+      <c r="A28" s="23" t="s">
+        <v>116</v>
+      </c>
+      <c r="B28" s="23" t="s">
+        <v>115</v>
+      </c>
+      <c r="C28" s="23" t="s">
         <v>14</v>
       </c>
-      <c r="D28" s="26" t="s">
-        <v>137</v>
-      </c>
-      <c r="E28" s="26" t="s">
+      <c r="D28" s="24" t="s">
+        <v>130</v>
+      </c>
+      <c r="E28" s="24" t="s">
         <v>88</v>
       </c>
-      <c r="F28" s="26" t="s">
+      <c r="F28" s="24" t="s">
         <v>90</v>
       </c>
-      <c r="G28" s="27" t="s">
+      <c r="G28" s="25" t="s">
         <v>87</v>
       </c>
       <c r="H28" s="4"/>
@@ -2673,7 +2658,7 @@
         <v>33</v>
       </c>
       <c r="E29" s="11" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="F29" s="11" t="s">
         <v>86</v>
@@ -2688,13 +2673,13 @@
         <v>20</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>131</v>
+        <v>124</v>
       </c>
       <c r="C30" s="7" t="s">
         <v>82</v>
       </c>
       <c r="D30" s="7" t="s">
-        <v>140</v>
+        <v>133</v>
       </c>
       <c r="E30" s="11" t="s">
         <v>99</v>
@@ -2712,16 +2697,16 @@
         <v>21</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>150</v>
+        <v>142</v>
       </c>
       <c r="C31" s="7" t="s">
         <v>32</v>
       </c>
       <c r="D31" s="7" t="s">
-        <v>149</v>
+        <v>141</v>
       </c>
       <c r="E31" s="11" t="s">
-        <v>132</v>
+        <v>125</v>
       </c>
       <c r="F31" s="11" t="s">
         <v>86</v>
@@ -2736,7 +2721,7 @@
         <v>22</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>151</v>
+        <v>143</v>
       </c>
       <c r="C32" s="7" t="s">
         <v>83</v>
@@ -2760,7 +2745,7 @@
         <v>23</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>152</v>
+        <v>144</v>
       </c>
       <c r="C33" s="7" t="s">
         <v>32</v>
@@ -2769,7 +2754,7 @@
         <v>24</v>
       </c>
       <c r="E33" s="11" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="F33" s="11" t="s">
         <v>86</v>
@@ -2784,7 +2769,7 @@
         <v>24</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>153</v>
+        <v>145</v>
       </c>
       <c r="C34" s="7" t="s">
         <v>32</v>
@@ -2793,7 +2778,7 @@
         <v>27</v>
       </c>
       <c r="E34" s="11" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="F34" s="11" t="s">
         <v>86</v>
@@ -2808,16 +2793,16 @@
         <v>25</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>154</v>
+        <v>146</v>
       </c>
       <c r="C35" s="7" t="s">
         <v>32</v>
       </c>
       <c r="D35" s="7" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="E35" s="11" t="s">
-        <v>155</v>
+        <v>147</v>
       </c>
       <c r="F35" s="11" t="s">
         <v>86</v>
@@ -2832,7 +2817,7 @@
         <v>26</v>
       </c>
       <c r="B36" s="11" t="s">
-        <v>133</v>
+        <v>126</v>
       </c>
       <c r="C36" s="11" t="s">
         <v>32</v>
@@ -2862,10 +2847,10 @@
         <v>82</v>
       </c>
       <c r="D37" s="11" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
       <c r="E37" s="1" t="s">
-        <v>102</v>
+        <v>148</v>
       </c>
       <c r="F37" s="1" t="s">
         <v>86</v>
@@ -2889,10 +2874,10 @@
         <v>21</v>
       </c>
       <c r="E38" s="1" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="F38" s="1" t="s">
-        <v>141</v>
+        <v>134</v>
       </c>
       <c r="G38" s="1" t="s">
         <v>98</v>
@@ -2913,7 +2898,7 @@
         <v>22</v>
       </c>
       <c r="E39" s="1" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="F39" s="1" t="s">
         <v>31</v>
@@ -2928,16 +2913,16 @@
         <v>30</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C40" s="7" t="s">
         <v>32</v>
       </c>
       <c r="D40" s="7" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="E40" s="11" t="s">
-        <v>109</v>
+        <v>149</v>
       </c>
       <c r="F40" s="1" t="s">
         <v>48</v>
@@ -2995,7 +2980,7 @@
       </c>
       <c r="H42" s="9"/>
     </row>
-    <row r="43" spans="1:8" ht="18">
+    <row r="43" spans="1:8" ht="16.5">
       <c r="A43" s="3">
         <v>33</v>
       </c>
@@ -3003,7 +2988,7 @@
         <v>30</v>
       </c>
       <c r="C43" s="7" t="s">
-        <v>82</v>
+        <v>32</v>
       </c>
       <c r="D43" s="7" t="s">
         <v>46</v>
@@ -3036,14 +3021,14 @@
         <v>32</v>
       </c>
       <c r="F44" s="1" t="s">
-        <v>139</v>
+        <v>132</v>
       </c>
       <c r="G44" s="1" t="s">
         <v>98</v>
       </c>
       <c r="H44" s="9"/>
     </row>
-    <row r="45" spans="1:8" ht="18">
+    <row r="45" spans="1:8" ht="16.5">
       <c r="A45" s="3">
         <v>35</v>
       </c>
@@ -3051,7 +3036,7 @@
         <v>29</v>
       </c>
       <c r="C45" s="7" t="s">
-        <v>82</v>
+        <v>32</v>
       </c>
       <c r="D45" s="7" t="s">
         <v>47</v>
@@ -3072,19 +3057,19 @@
         <v>36</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>134</v>
+        <v>127</v>
       </c>
       <c r="C46" s="7" t="s">
         <v>84</v>
       </c>
       <c r="D46" s="7" t="s">
-        <v>138</v>
+        <v>131</v>
       </c>
       <c r="E46" s="1" t="s">
-        <v>135</v>
+        <v>128</v>
       </c>
       <c r="F46" s="1" t="s">
-        <v>136</v>
+        <v>129</v>
       </c>
       <c r="G46" s="1" t="s">
         <v>98</v>
@@ -3105,10 +3090,10 @@
         <v>26</v>
       </c>
       <c r="E47" s="1" t="s">
-        <v>143</v>
+        <v>150</v>
       </c>
       <c r="F47" s="1" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="G47" s="1" t="s">
         <v>98</v>
@@ -3120,19 +3105,19 @@
         <v>38</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>120</v>
+        <v>113</v>
       </c>
       <c r="C48" s="7" t="s">
         <v>2</v>
       </c>
       <c r="D48" s="7" t="s">
-        <v>121</v>
+        <v>114</v>
       </c>
       <c r="E48" s="11" t="s">
         <v>32</v>
       </c>
       <c r="F48" s="11" t="s">
-        <v>142</v>
+        <v>135</v>
       </c>
       <c r="G48" s="1" t="s">
         <v>98</v>
@@ -3180,7 +3165,7 @@
         <v>74</v>
       </c>
       <c r="F50" s="1" t="s">
-        <v>144</v>
+        <v>136</v>
       </c>
       <c r="G50" s="1" t="s">
         <v>98</v>
@@ -3191,20 +3176,20 @@
       <c r="A51" s="3">
         <v>41</v>
       </c>
-      <c r="B51" s="17" t="s">
+      <c r="B51" s="35" t="s">
         <v>58</v>
       </c>
-      <c r="C51" s="17" t="s">
+      <c r="C51" s="35" t="s">
         <v>2</v>
       </c>
-      <c r="D51" s="17" t="s">
+      <c r="D51" s="35" t="s">
         <v>45</v>
       </c>
-      <c r="E51" s="18" t="s">
-        <v>118</v>
-      </c>
-      <c r="F51" s="18" t="s">
-        <v>119</v>
+      <c r="E51" s="36" t="s">
+        <v>151</v>
+      </c>
+      <c r="F51" s="36" t="s">
+        <v>152</v>
       </c>
       <c r="G51" s="1" t="s">
         <v>98</v>
@@ -3215,20 +3200,20 @@
       <c r="A52" s="3">
         <v>42</v>
       </c>
-      <c r="B52" s="17" t="s">
+      <c r="B52" s="35" t="s">
         <v>57</v>
       </c>
-      <c r="C52" s="17" t="s">
+      <c r="C52" s="35" t="s">
         <v>2</v>
       </c>
-      <c r="D52" s="17" t="s">
+      <c r="D52" s="35" t="s">
         <v>40</v>
       </c>
-      <c r="E52" s="18" t="s">
-        <v>118</v>
-      </c>
-      <c r="F52" s="18" t="s">
-        <v>117</v>
+      <c r="E52" s="36" t="s">
+        <v>151</v>
+      </c>
+      <c r="F52" s="36" t="s">
+        <v>153</v>
       </c>
       <c r="G52" s="1" t="s">
         <v>98</v>
@@ -3276,7 +3261,7 @@
         <v>32</v>
       </c>
       <c r="F54" s="1" t="s">
-        <v>112</v>
+        <v>154</v>
       </c>
       <c r="G54" s="1" t="s">
         <v>98</v>
@@ -3300,7 +3285,7 @@
         <v>32</v>
       </c>
       <c r="F55" s="1" t="s">
-        <v>113</v>
+        <v>155</v>
       </c>
       <c r="G55" s="1" t="s">
         <v>98</v>
@@ -3321,7 +3306,7 @@
         <v>61</v>
       </c>
       <c r="E56" s="1" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="F56" s="1" t="s">
         <v>28</v>

</xml_diff>

<commit_message>
Some renames in yesterday works. it is compiles now but test suit is not complete yet
</commit_message>
<xml_diff>
--- a/stm/documents/algorithm_and_tests/Short_Variable_List_Sediment_Version_02_10_11_version_2.xlsx
+++ b/stm/documents/algorithm_and_tests/Short_Variable_List_Sediment_Version_02_10_11_version_2.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="259" uniqueCount="156">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="269" uniqueCount="160">
   <si>
     <t>Gravitational acceleration</t>
   </si>
@@ -1466,6 +1466,18 @@
       </rPr>
       <t>s</t>
     </r>
+  </si>
+  <si>
+    <t>*</t>
+  </si>
+  <si>
+    <t>????</t>
+  </si>
+  <si>
+    <t>same as non-cohesive + correction factor</t>
+  </si>
+  <si>
+    <t>equation 4.1.11 Van Rijn Book (Yalin 1972)</t>
   </si>
 </sst>
 </file>
@@ -1734,7 +1746,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="37">
+  <cellXfs count="38">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1815,6 +1827,12 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -1824,12 +1842,7 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2127,7 +2140,7 @@
   <dimension ref="A1:O56"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="G61" sqref="G61"/>
+      <selection activeCell="H20" sqref="H20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2163,22 +2176,22 @@
       <c r="O1" s="6"/>
     </row>
     <row r="2" spans="1:15" ht="132.75" customHeight="1">
-      <c r="B2" s="34" t="s">
+      <c r="B2" s="36" t="s">
         <v>119</v>
       </c>
-      <c r="C2" s="34"/>
-      <c r="D2" s="34"/>
-      <c r="E2" s="34"/>
-      <c r="F2" s="34"/>
-      <c r="G2" s="34"/>
-      <c r="H2" s="34"/>
-      <c r="I2" s="34"/>
-      <c r="J2" s="34"/>
-      <c r="K2" s="34"/>
-      <c r="L2" s="34"/>
-      <c r="M2" s="34"/>
-      <c r="N2" s="34"/>
-      <c r="O2" s="34"/>
+      <c r="C2" s="36"/>
+      <c r="D2" s="36"/>
+      <c r="E2" s="36"/>
+      <c r="F2" s="36"/>
+      <c r="G2" s="36"/>
+      <c r="H2" s="36"/>
+      <c r="I2" s="36"/>
+      <c r="J2" s="36"/>
+      <c r="K2" s="36"/>
+      <c r="L2" s="36"/>
+      <c r="M2" s="36"/>
+      <c r="N2" s="36"/>
+      <c r="O2" s="36"/>
     </row>
     <row r="3" spans="1:15" ht="19.5" thickBot="1">
       <c r="A3" s="17" t="s">
@@ -2579,26 +2592,26 @@
       <c r="H23" s="4"/>
     </row>
     <row r="24" spans="1:8">
-      <c r="A24" s="32" t="s">
+      <c r="A24" s="34" t="s">
         <v>118</v>
       </c>
-      <c r="B24" s="33"/>
-      <c r="C24" s="33"/>
-      <c r="D24" s="33"/>
-      <c r="E24" s="33"/>
-      <c r="F24" s="33"/>
+      <c r="B24" s="35"/>
+      <c r="C24" s="35"/>
+      <c r="D24" s="35"/>
+      <c r="E24" s="35"/>
+      <c r="F24" s="35"/>
       <c r="G24" s="4"/>
       <c r="H24" s="4"/>
     </row>
     <row r="25" spans="1:8">
-      <c r="A25" s="32" t="s">
+      <c r="A25" s="34" t="s">
         <v>117</v>
       </c>
-      <c r="B25" s="33"/>
-      <c r="C25" s="33"/>
-      <c r="D25" s="33"/>
-      <c r="E25" s="33"/>
-      <c r="F25" s="33"/>
+      <c r="B25" s="35"/>
+      <c r="C25" s="35"/>
+      <c r="D25" s="35"/>
+      <c r="E25" s="35"/>
+      <c r="F25" s="35"/>
       <c r="G25" s="4"/>
       <c r="H25" s="4"/>
     </row>
@@ -2666,7 +2679,9 @@
       <c r="G29" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="H29" s="9"/>
+      <c r="H29" s="9" t="s">
+        <v>156</v>
+      </c>
     </row>
     <row r="30" spans="1:8" ht="18">
       <c r="A30" s="3">
@@ -2690,7 +2705,9 @@
       <c r="G30" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="H30" s="9"/>
+      <c r="H30" s="27" t="s">
+        <v>156</v>
+      </c>
     </row>
     <row r="31" spans="1:8" ht="16.5">
       <c r="A31" s="3">
@@ -2714,7 +2731,9 @@
       <c r="G31" s="11" t="s">
         <v>32</v>
       </c>
-      <c r="H31" s="4"/>
+      <c r="H31" s="4" t="s">
+        <v>156</v>
+      </c>
     </row>
     <row r="32" spans="1:8" ht="18">
       <c r="A32" s="3">
@@ -2738,9 +2757,11 @@
       <c r="G32" s="11" t="s">
         <v>32</v>
       </c>
-      <c r="H32" s="4"/>
-    </row>
-    <row r="33" spans="1:8" ht="16.5">
+      <c r="H32" s="4" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9" ht="16.5">
       <c r="A33" s="3">
         <v>23</v>
       </c>
@@ -2762,9 +2783,11 @@
       <c r="G33" s="11" t="s">
         <v>32</v>
       </c>
-      <c r="H33" s="4"/>
-    </row>
-    <row r="34" spans="1:8" ht="16.5">
+      <c r="H33" s="4" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9" ht="16.5">
       <c r="A34" s="3">
         <v>24</v>
       </c>
@@ -2786,9 +2809,11 @@
       <c r="G34" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="H34" s="9"/>
-    </row>
-    <row r="35" spans="1:8" ht="16.5">
+      <c r="H34" s="9" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9" ht="16.5">
       <c r="A35" s="3">
         <v>25</v>
       </c>
@@ -2810,9 +2835,14 @@
       <c r="G35" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="H35" s="9"/>
-    </row>
-    <row r="36" spans="1:8" ht="16.5">
+      <c r="H35" s="27" t="s">
+        <v>157</v>
+      </c>
+      <c r="I35" s="37" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9" ht="16.5">
       <c r="A36" s="3">
         <v>26</v>
       </c>
@@ -2834,9 +2864,11 @@
       <c r="G36" s="11" t="s">
         <v>32</v>
       </c>
-      <c r="H36" s="4"/>
-    </row>
-    <row r="37" spans="1:8" ht="18">
+      <c r="H36" s="4" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9" ht="30">
       <c r="A37" s="3">
         <v>27</v>
       </c>
@@ -2858,9 +2890,11 @@
       <c r="G37" s="11" t="s">
         <v>32</v>
       </c>
-      <c r="H37" s="4"/>
-    </row>
-    <row r="38" spans="1:8" ht="17.25" customHeight="1">
+      <c r="H37" s="4" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9" ht="17.25" customHeight="1">
       <c r="A38" s="3">
         <v>28</v>
       </c>
@@ -2884,7 +2918,7 @@
       </c>
       <c r="H38" s="9"/>
     </row>
-    <row r="39" spans="1:8" ht="17.25" customHeight="1">
+    <row r="39" spans="1:9" ht="17.25" customHeight="1">
       <c r="A39" s="3">
         <v>29</v>
       </c>
@@ -2908,7 +2942,7 @@
       </c>
       <c r="H39" s="9"/>
     </row>
-    <row r="40" spans="1:8" ht="17.25" customHeight="1">
+    <row r="40" spans="1:9" ht="17.25" customHeight="1">
       <c r="A40" s="3">
         <v>30</v>
       </c>
@@ -2932,7 +2966,7 @@
       </c>
       <c r="H40" s="9"/>
     </row>
-    <row r="41" spans="1:8" ht="17.25" customHeight="1">
+    <row r="41" spans="1:9" ht="17.25" customHeight="1">
       <c r="A41" s="3">
         <v>31</v>
       </c>
@@ -2956,7 +2990,7 @@
       </c>
       <c r="H41" s="9"/>
     </row>
-    <row r="42" spans="1:8" ht="16.5">
+    <row r="42" spans="1:9" ht="16.5">
       <c r="A42" s="3">
         <v>32</v>
       </c>
@@ -2980,7 +3014,7 @@
       </c>
       <c r="H42" s="9"/>
     </row>
-    <row r="43" spans="1:8" ht="16.5">
+    <row r="43" spans="1:9" ht="16.5">
       <c r="A43" s="3">
         <v>33</v>
       </c>
@@ -3004,7 +3038,7 @@
       </c>
       <c r="H43" s="9"/>
     </row>
-    <row r="44" spans="1:8" ht="16.5">
+    <row r="44" spans="1:9" ht="16.5">
       <c r="A44" s="3">
         <v>34</v>
       </c>
@@ -3028,7 +3062,7 @@
       </c>
       <c r="H44" s="9"/>
     </row>
-    <row r="45" spans="1:8" ht="16.5">
+    <row r="45" spans="1:9" ht="16.5">
       <c r="A45" s="3">
         <v>35</v>
       </c>
@@ -3052,7 +3086,7 @@
       </c>
       <c r="H45" s="4"/>
     </row>
-    <row r="46" spans="1:8" ht="18">
+    <row r="46" spans="1:9" ht="18">
       <c r="A46" s="3">
         <v>36</v>
       </c>
@@ -3076,7 +3110,7 @@
       </c>
       <c r="H46" s="4"/>
     </row>
-    <row r="47" spans="1:8" ht="16.5">
+    <row r="47" spans="1:9" ht="16.5">
       <c r="A47" s="3">
         <v>37</v>
       </c>
@@ -3100,7 +3134,7 @@
       </c>
       <c r="H47" s="9"/>
     </row>
-    <row r="48" spans="1:8" ht="16.5" customHeight="1">
+    <row r="48" spans="1:9" ht="16.5" customHeight="1">
       <c r="A48" s="3">
         <v>38</v>
       </c>
@@ -3176,19 +3210,19 @@
       <c r="A51" s="3">
         <v>41</v>
       </c>
-      <c r="B51" s="35" t="s">
+      <c r="B51" s="32" t="s">
         <v>58</v>
       </c>
-      <c r="C51" s="35" t="s">
+      <c r="C51" s="32" t="s">
         <v>2</v>
       </c>
-      <c r="D51" s="35" t="s">
+      <c r="D51" s="32" t="s">
         <v>45</v>
       </c>
-      <c r="E51" s="36" t="s">
+      <c r="E51" s="33" t="s">
         <v>151</v>
       </c>
-      <c r="F51" s="36" t="s">
+      <c r="F51" s="33" t="s">
         <v>152</v>
       </c>
       <c r="G51" s="1" t="s">
@@ -3200,19 +3234,19 @@
       <c r="A52" s="3">
         <v>42</v>
       </c>
-      <c r="B52" s="35" t="s">
+      <c r="B52" s="32" t="s">
         <v>57</v>
       </c>
-      <c r="C52" s="35" t="s">
+      <c r="C52" s="32" t="s">
         <v>2</v>
       </c>
-      <c r="D52" s="35" t="s">
+      <c r="D52" s="32" t="s">
         <v>40</v>
       </c>
-      <c r="E52" s="36" t="s">
+      <c r="E52" s="33" t="s">
         <v>151</v>
       </c>
-      <c r="F52" s="36" t="s">
+      <c r="F52" s="33" t="s">
         <v>153</v>
       </c>
       <c r="G52" s="1" t="s">

</xml_diff>

<commit_message>
Some cleaning and commenting of files of the sediment part.
</commit_message>
<xml_diff>
--- a/stm/documents/algorithm_and_tests/Short_Variable_List_Sediment_Version_02_10_11_version_2.xlsx
+++ b/stm/documents/algorithm_and_tests/Short_Variable_List_Sediment_Version_02_10_11_version_2.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="269" uniqueCount="160">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="279" uniqueCount="160">
   <si>
     <t>Gravitational acceleration</t>
   </si>
@@ -1833,6 +1833,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -1842,7 +1843,6 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2139,8 +2139,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:O56"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="H20" sqref="H20"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2175,23 +2175,23 @@
       <c r="N1" s="6"/>
       <c r="O1" s="6"/>
     </row>
-    <row r="2" spans="1:15" ht="132.75" customHeight="1">
-      <c r="B2" s="36" t="s">
+    <row r="2" spans="1:15" ht="80.25" customHeight="1">
+      <c r="B2" s="37" t="s">
         <v>119</v>
       </c>
-      <c r="C2" s="36"/>
-      <c r="D2" s="36"/>
-      <c r="E2" s="36"/>
-      <c r="F2" s="36"/>
-      <c r="G2" s="36"/>
-      <c r="H2" s="36"/>
-      <c r="I2" s="36"/>
-      <c r="J2" s="36"/>
-      <c r="K2" s="36"/>
-      <c r="L2" s="36"/>
-      <c r="M2" s="36"/>
-      <c r="N2" s="36"/>
-      <c r="O2" s="36"/>
+      <c r="C2" s="37"/>
+      <c r="D2" s="37"/>
+      <c r="E2" s="37"/>
+      <c r="F2" s="37"/>
+      <c r="G2" s="37"/>
+      <c r="H2" s="37"/>
+      <c r="I2" s="37"/>
+      <c r="J2" s="37"/>
+      <c r="K2" s="37"/>
+      <c r="L2" s="37"/>
+      <c r="M2" s="37"/>
+      <c r="N2" s="37"/>
+      <c r="O2" s="37"/>
     </row>
     <row r="3" spans="1:15" ht="19.5" thickBot="1">
       <c r="A3" s="17" t="s">
@@ -2237,7 +2237,9 @@
       <c r="E5" s="10" t="s">
         <v>86</v>
       </c>
-      <c r="F5" s="27"/>
+      <c r="F5" s="27" t="s">
+        <v>156</v>
+      </c>
       <c r="G5" s="4"/>
       <c r="H5" s="4"/>
     </row>
@@ -2257,7 +2259,9 @@
       <c r="E6" s="10" t="s">
         <v>86</v>
       </c>
-      <c r="F6" s="28"/>
+      <c r="F6" s="28" t="s">
+        <v>156</v>
+      </c>
       <c r="G6" s="4"/>
       <c r="H6" s="4"/>
     </row>
@@ -2277,7 +2281,9 @@
       <c r="E7" s="10" t="s">
         <v>100</v>
       </c>
-      <c r="F7" s="27"/>
+      <c r="F7" s="27" t="s">
+        <v>156</v>
+      </c>
       <c r="G7" s="4"/>
       <c r="H7" s="4"/>
     </row>
@@ -2297,7 +2303,9 @@
       <c r="E8" s="10" t="s">
         <v>101</v>
       </c>
-      <c r="F8" s="27"/>
+      <c r="F8" s="27" t="s">
+        <v>156</v>
+      </c>
       <c r="G8" s="4"/>
       <c r="H8" s="4"/>
     </row>
@@ -2317,7 +2325,9 @@
       <c r="E9" s="10" t="s">
         <v>86</v>
       </c>
-      <c r="F9" s="27"/>
+      <c r="F9" s="27" t="s">
+        <v>156</v>
+      </c>
       <c r="G9" s="4"/>
       <c r="H9" s="4"/>
     </row>
@@ -2337,7 +2347,9 @@
       <c r="E10" s="10" t="s">
         <v>86</v>
       </c>
-      <c r="F10" s="27"/>
+      <c r="F10" s="27" t="s">
+        <v>156</v>
+      </c>
       <c r="G10" s="4"/>
       <c r="H10" s="4"/>
     </row>
@@ -2357,7 +2369,9 @@
       <c r="E11" s="10" t="s">
         <v>86</v>
       </c>
-      <c r="F11" s="27"/>
+      <c r="F11" s="27" t="s">
+        <v>156</v>
+      </c>
       <c r="G11" s="4"/>
       <c r="H11" s="4"/>
     </row>
@@ -2377,7 +2391,9 @@
       <c r="E12" s="10" t="s">
         <v>86</v>
       </c>
-      <c r="F12" s="27"/>
+      <c r="F12" s="27" t="s">
+        <v>156</v>
+      </c>
       <c r="G12" s="4"/>
       <c r="H12" s="4"/>
     </row>
@@ -2397,7 +2413,9 @@
       <c r="E13" s="8" t="s">
         <v>86</v>
       </c>
-      <c r="F13" s="27"/>
+      <c r="F13" s="27" t="s">
+        <v>156</v>
+      </c>
       <c r="G13" s="9"/>
       <c r="H13" s="9"/>
     </row>
@@ -2417,7 +2435,9 @@
       <c r="E14" s="8" t="s">
         <v>105</v>
       </c>
-      <c r="F14" s="27"/>
+      <c r="F14" s="27" t="s">
+        <v>156</v>
+      </c>
       <c r="G14" s="9"/>
       <c r="H14" s="9"/>
     </row>
@@ -2592,26 +2612,26 @@
       <c r="H23" s="4"/>
     </row>
     <row r="24" spans="1:8">
-      <c r="A24" s="34" t="s">
+      <c r="A24" s="35" t="s">
         <v>118</v>
       </c>
-      <c r="B24" s="35"/>
-      <c r="C24" s="35"/>
-      <c r="D24" s="35"/>
-      <c r="E24" s="35"/>
-      <c r="F24" s="35"/>
+      <c r="B24" s="36"/>
+      <c r="C24" s="36"/>
+      <c r="D24" s="36"/>
+      <c r="E24" s="36"/>
+      <c r="F24" s="36"/>
       <c r="G24" s="4"/>
       <c r="H24" s="4"/>
     </row>
     <row r="25" spans="1:8">
-      <c r="A25" s="34" t="s">
+      <c r="A25" s="35" t="s">
         <v>117</v>
       </c>
-      <c r="B25" s="35"/>
-      <c r="C25" s="35"/>
-      <c r="D25" s="35"/>
-      <c r="E25" s="35"/>
-      <c r="F25" s="35"/>
+      <c r="B25" s="36"/>
+      <c r="C25" s="36"/>
+      <c r="D25" s="36"/>
+      <c r="E25" s="36"/>
+      <c r="F25" s="36"/>
       <c r="G25" s="4"/>
       <c r="H25" s="4"/>
     </row>
@@ -2838,7 +2858,7 @@
       <c r="H35" s="27" t="s">
         <v>157</v>
       </c>
-      <c r="I35" s="37" t="s">
+      <c r="I35" s="34" t="s">
         <v>159</v>
       </c>
     </row>

</xml_diff>